<commit_message>
Adding a new place to the stats and updating the dashboards
</commit_message>
<xml_diff>
--- a/erv_table.xlsx
+++ b/erv_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BASE\Code\Erv_places_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA1D3D3-CFBF-44D6-A5A6-7BAE96DC6CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4447D2-4563-43D6-8335-313108D0A722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>PLACE_NAME</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>POSITION</t>
+  </si>
+  <si>
+    <t>Apartment Sayat-Nova 18</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,6 +597,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>40.181066166026902</v>
+      </c>
+      <c r="F9">
+        <v>44.521552090821501</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding another new place
</commit_message>
<xml_diff>
--- a/erv_table.xlsx
+++ b/erv_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BASE\Code\Erv_places_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4447D2-4563-43D6-8335-313108D0A722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A46C5-3F57-43BD-B48F-7A62E0A232D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>PLACE_NAME</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Apartment Sayat-Nova 18</t>
+  </si>
+  <si>
+    <t>Apartment at Sayat-Nova Street</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,6 +623,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>40.169242536025401</v>
+      </c>
+      <c r="F10">
+        <v>44.5038657799916</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding our 10th place here
</commit_message>
<xml_diff>
--- a/erv_table.xlsx
+++ b/erv_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BASE\Code\Erv_places_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A46C5-3F57-43BD-B48F-7A62E0A232D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4E4F3E-F91D-4D9F-878D-7370CBC332BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>PLACE_NAME</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Apartment at Sayat-Nova Street</t>
+  </si>
+  <si>
+    <t>Cosy Studio with Beautiful Garden</t>
+  </si>
+  <si>
+    <t>Nork-Marash</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +652,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>40.181362719104797</v>
+      </c>
+      <c r="F11">
+        <v>44.531758099622301</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding a new place near the Cascade
</commit_message>
<xml_diff>
--- a/erv_table.xlsx
+++ b/erv_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BASE\Code\Erv_places_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4E4F3E-F91D-4D9F-878D-7370CBC332BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5BAC80-C9C2-4D67-8A23-5B8278B534D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>PLACE_NAME</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Nork-Marash</t>
+  </si>
+  <si>
+    <t>Cozy Apartments Near Cascade In DownTown</t>
   </si>
 </sst>
 </file>
@@ -414,13 +417,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -675,6 +681,29 @@
         <v>23</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>40.191701778676297</v>
+      </c>
+      <c r="F12">
+        <v>44.517007512745899</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding a new place in Arabkir
</commit_message>
<xml_diff>
--- a/erv_table.xlsx
+++ b/erv_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BASE\Code\Erv_places_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5BAC80-C9C2-4D67-8A23-5B8278B534D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDC9E6B-896D-4AA9-8A32-3D8793D67DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>PLACE_NAME</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Cozy Apartments Near Cascade In DownTown</t>
+  </si>
+  <si>
+    <t>Appartments</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,6 +707,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>40.204659150041699</v>
+      </c>
+      <c r="F13">
+        <v>44.520428336322297</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding the 14th place
</commit_message>
<xml_diff>
--- a/erv_table.xlsx
+++ b/erv_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BASE\Code\Erv_places_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F445FED9-F9C7-46E5-8C2B-8061F57A68E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40E75C4-D3F8-446D-9769-1B7CD8A64E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>PLACE_NAME</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Amiryan Aprtament</t>
+  </si>
+  <si>
+    <t>Yerevan, Artsakh Street</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,6 +759,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>40.144787358096401</v>
+      </c>
+      <c r="F15">
+        <v>44.510079586555797</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding 15th place (coliving)
</commit_message>
<xml_diff>
--- a/erv_table.xlsx
+++ b/erv_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BASE\Code\Erv_places_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40E75C4-D3F8-446D-9769-1B7CD8A64E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE7FE87-8CE8-472E-BFCF-9347EE2CE976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>PLACE_NAME</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Yerevan, Artsakh Street</t>
+  </si>
+  <si>
+    <t>Arinj Coliving</t>
+  </si>
+  <si>
+    <t>Coliving</t>
+  </si>
+  <si>
+    <t>Avan</t>
   </si>
 </sst>
 </file>
@@ -426,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,6 +791,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>40.232358277056797</v>
+      </c>
+      <c r="F16">
+        <v>44.570450348513901</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>